<commit_message>
The build and task progress
</commit_message>
<xml_diff>
--- a/Build/TaskList.xlsx
+++ b/Build/TaskList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>If the image has the path "&lt;C://images/Backgrounds/Guitars/Fender/Sonic&gt; Blue Telecaster.png", and the "&lt;C://images/Backgrounds&gt;" was opened by the app and "Guitars" subcategory is selected right now, then it should be found by any of the words in the list "Fender, Sonic, Blue, Telecaster".</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>In progress</t>
-  </si>
-  <si>
-    <t>Not started</t>
   </si>
   <si>
     <t>Completed</t>
@@ -156,7 +153,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -168,20 +165,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -515,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -534,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" customHeight="1">
@@ -548,7 +531,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" customHeight="1">
@@ -562,7 +545,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" customHeight="1">
@@ -573,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" customHeight="1">
@@ -595,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" customHeight="1">
@@ -606,10 +589,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" customHeight="1">
@@ -620,10 +603,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" customHeight="1">
@@ -634,10 +617,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" customHeight="1">
@@ -681,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" customHeight="1">
@@ -703,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" customHeight="1">

</xml_diff>

<commit_message>
Some more performance fixes, a bit of decoration for not loaded thumbnails and the Windows build
</commit_message>
<xml_diff>
--- a/Build/TaskList.xlsx
+++ b/Build/TaskList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>If the image has the path "&lt;C://images/Backgrounds/Guitars/Fender/Sonic&gt; Blue Telecaster.png", and the "&lt;C://images/Backgrounds&gt;" was opened by the app and "Guitars" subcategory is selected right now, then it should be found by any of the words in the list "Fender, Sonic, Blue, Telecaster".</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>The menu is dummy</t>
+  </si>
+  <si>
+    <t>Root directory is defined by --setrootfolder=[dir] and is ignored by --filesystem</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -496,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -542,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
@@ -567,7 +598,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" customHeight="1">
@@ -700,18 +731,37 @@
         <v>18</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:C1"/>
   <conditionalFormatting sqref="C2:C16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Completed">
+      <formula>NOT(ISERROR(SEARCH("Completed",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C16">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C17">
       <formula1>"Not started, In progress, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>